<commit_message>
09/08/2018 RUP - DSDM
</commit_message>
<xml_diff>
--- a/Pasantía/Requisitos.xlsx
+++ b/Pasantía/Requisitos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mannuel\Documents\Pasantía\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mannuel\Documents\OpenHeadoCount\Pasantía\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2841B045-491E-4481-85D3-297EB916113E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="2" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="82">
   <si>
     <t>1.0</t>
   </si>
@@ -254,12 +255,24 @@
   </si>
   <si>
     <t>El sistema actual cuenta con un formulario para la actualización de la información del empleado, pero la consulta de esta infomación es compleja.</t>
+  </si>
+  <si>
+    <t>UR-006</t>
+  </si>
+  <si>
+    <t>Formulario para el registro</t>
+  </si>
+  <si>
+    <t>Se requiere que el formulario para el registro y visualización de la información sea personalizable por roles de usuario.</t>
+  </si>
+  <si>
+    <t>Manuel Quesada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -599,7 +612,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Sage Pivot Table Style" count="0"/>
+    <tableStyle name="Sage Pivot Table Style" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -996,7 +1009,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1450,7 +1463,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1770,21 +1783,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A18:L50" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A18:L50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A18:L50" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A18:L50" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="ID" dataDxfId="11"/>
-    <tableColumn id="2" name="Título" dataDxfId="10"/>
-    <tableColumn id="12" name="Tipo" dataDxfId="9"/>
-    <tableColumn id="3" name="Descripción" dataDxfId="8"/>
-    <tableColumn id="4" name="Razón" dataDxfId="7"/>
-    <tableColumn id="5" name="Creado por" dataDxfId="6"/>
-    <tableColumn id="6" name="Fuente" dataDxfId="5"/>
-    <tableColumn id="7" name="Asignación" dataDxfId="4"/>
-    <tableColumn id="8" name="Requisitos relacionados" dataDxfId="3"/>
-    <tableColumn id="11" name="Estado" dataDxfId="2"/>
-    <tableColumn id="9" name="Complejidad" dataDxfId="1"/>
-    <tableColumn id="10" name="Impacto en el negocio" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Título" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Tipo" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Descripción" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Razón" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Creado por" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Fuente" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Asignación" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Requisitos relacionados" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Estado" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Complejidad" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Impacto en el negocio" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2110,11 +2123,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A6:D34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
@@ -2143,7 +2156,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>37</v>
       </c>
@@ -2170,7 +2183,7 @@
       </c>
       <c r="C14">
         <f>COUNTA(Tabla1[ID])</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2218,7 +2231,7 @@
       </c>
       <c r="C19">
         <f>COUNTIF(Requirements!$C$19:$C$50,Dashboard!B19)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2303,7 +2316,7 @@
       </c>
       <c r="C28">
         <f>COUNTIF(Requirements!$J$19:$J$50,Dashboard!B28)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2374,12 +2387,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2790,19 +2803,35 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+    <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="F24" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
+      <c r="J24" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
@@ -3171,16 +3200,16 @@
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K20:L50 K19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K20:L50 K19" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$O$2:$O$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J19:J50">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J19:J50" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$P$2:$P$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C51:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C51:C1048576" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>$Q$2:$Q$9</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:C50">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:C50" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>$Q$2:$Q$12</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>